<commit_message>
last work to push
</commit_message>
<xml_diff>
--- a/M100/IC-Basic-SWOT-Matrix-Template-8629.xlsx
+++ b/M100/IC-Basic-SWOT-Matrix-Template-8629.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\uni_masters\M100\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\uni_masters\M100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6B3A1A0-BE90-4691-9103-97D7A137B214}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0E581-C04D-4C06-93D1-B511BD0A2E6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic SWOT Matrix" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>INTERNAL FACTORS</t>
   </si>
@@ -62,6 +61,78 @@
   </si>
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
+  </si>
+  <si>
+    <t>Continuous Improvement Model, Digital dashbord, company performance</t>
+  </si>
+  <si>
+    <t>New Innovation</t>
+  </si>
+  <si>
+    <t>500,000 sq ft of secure UK centric, high quality warehousing</t>
+  </si>
+  <si>
+    <t>Currently use Transormational leadership</t>
+  </si>
+  <si>
+    <t>Brexit</t>
+  </si>
+  <si>
+    <t>Global warming</t>
+  </si>
+  <si>
+    <t>Import Export around the world, Good reach of advertisement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Believe Employee empowerment </t>
+  </si>
+  <si>
+    <t>Implement Agile methodologies</t>
+  </si>
+  <si>
+    <t>Communication seems to only go from top down</t>
+  </si>
+  <si>
+    <t>Driverless cars</t>
+  </si>
+  <si>
+    <t>There will always be a demand for waerhousing</t>
+  </si>
+  <si>
+    <t>Strong interaction with customers</t>
+  </si>
+  <si>
+    <t>Communication barrier with multi cultural work force</t>
+  </si>
+  <si>
+    <t>News letters around the company</t>
+  </si>
+  <si>
+    <t>Organise family fun days</t>
+  </si>
+  <si>
+    <t>wars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tensions between the USA and China. Trade wars </t>
+  </si>
+  <si>
+    <t>29 years of experience</t>
+  </si>
+  <si>
+    <t>Carbon footprint</t>
+  </si>
+  <si>
+    <t>Whare house's can be viewed as eye sores and unnatural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Brexit could increase trade from other countries </t>
+  </si>
+  <si>
+    <t>Good employee interaction</t>
+  </si>
+  <si>
+    <t>Un-attractive business</t>
   </si>
 </sst>
 </file>
@@ -708,33 +779,33 @@
   </sheetPr>
   <dimension ref="B1:P48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.25" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24" style="2" customWidth="1"/>
-    <col min="5" max="5" width="1.796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="57.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18" style="2" customWidth="1"/>
+    <col min="5" max="5" width="1.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="70.75" style="2" customWidth="1"/>
     <col min="8" max="8" width="24" style="2" customWidth="1"/>
-    <col min="9" max="9" width="3.296875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="2"/>
+    <col min="9" max="9" width="3.25" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="10" t="s">
         <v>0</v>
@@ -746,7 +817,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
         <v>1</v>
@@ -762,66 +833,84 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="16"/>
       <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="18"/>
       <c r="F5" s="12">
         <f>F4+1</f>
         <v>2</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="17" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <f t="shared" ref="B6:B23" si="0">B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="F6" s="13">
         <f t="shared" ref="F6:F23" si="1">F5+1</f>
         <v>3</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="D7" s="18"/>
       <c r="F7" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="19" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="16"/>
       <c r="F8" s="13">
         <f t="shared" si="1"/>
@@ -830,12 +919,14 @@
       <c r="G8" s="19"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="18"/>
       <c r="F9" s="12">
         <f t="shared" si="1"/>
@@ -844,13 +935,17 @@
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="16">
+        <v>2</v>
+      </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -858,12 +953,14 @@
       <c r="G10" s="19"/>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="18"/>
       <c r="F11" s="12">
         <f t="shared" si="1"/>
@@ -872,12 +969,14 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="D12" s="16"/>
       <c r="F12" s="13">
         <f t="shared" si="1"/>
@@ -886,13 +985,17 @@
       <c r="G12" s="19"/>
       <c r="H12" s="16"/>
     </row>
-    <row r="13" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
+      <c r="C13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
       <c r="F13" s="12">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -900,12 +1003,14 @@
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="16"/>
       <c r="F14" s="13">
         <f t="shared" si="1"/>
@@ -914,12 +1019,14 @@
       <c r="G14" s="19"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="F15" s="12">
         <f t="shared" si="1"/>
@@ -928,7 +1035,7 @@
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -942,7 +1049,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="16"/>
     </row>
-    <row r="17" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -956,7 +1063,7 @@
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -970,7 +1077,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -984,7 +1091,7 @@
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -998,7 +1105,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1012,7 +1119,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1026,7 +1133,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1040,8 +1147,8 @@
       <c r="G23" s="17"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="2:8" ht="10.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="10.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="22" t="s">
         <v>2</v>
@@ -1053,7 +1160,7 @@
       </c>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
         <v>3</v>
@@ -1069,47 +1176,59 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14">
         <v>1</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="D27" s="25"/>
       <c r="F27" s="14">
         <v>1</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="24">
         <f>B27+1</f>
         <v>2</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="26" t="s">
+        <v>20</v>
+      </c>
       <c r="D28" s="27"/>
       <c r="F28" s="24">
         <f>F27+1</f>
         <v>2</v>
       </c>
-      <c r="G28" s="26"/>
+      <c r="G28" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="H28" s="27"/>
     </row>
-    <row r="29" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14">
         <f t="shared" ref="B29:B46" si="2">B28+1</f>
         <v>3</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D29" s="25"/>
       <c r="F29" s="14">
         <f t="shared" ref="F29:F46" si="3">F28+1</f>
         <v>3</v>
       </c>
-      <c r="G29" s="19"/>
+      <c r="G29" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="H29" s="25"/>
     </row>
-    <row r="30" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1120,10 +1239,12 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="G30" s="26"/>
+      <c r="G30" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="H30" s="27"/>
     </row>
-    <row r="31" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1134,10 +1255,12 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="H31" s="25"/>
     </row>
-    <row r="32" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="24">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1151,7 +1274,7 @@
       <c r="G32" s="26"/>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1165,7 +1288,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="25"/>
     </row>
-    <row r="34" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="24">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1179,7 +1302,7 @@
       <c r="G34" s="26"/>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1193,7 +1316,7 @@
       <c r="G35" s="19"/>
       <c r="H35" s="25"/>
     </row>
-    <row r="36" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="24">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1207,7 +1330,7 @@
       <c r="G36" s="26"/>
       <c r="H36" s="27"/>
     </row>
-    <row r="37" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="13">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1221,7 +1344,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="25"/>
     </row>
-    <row r="38" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="24">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1235,7 +1358,7 @@
       <c r="G38" s="26"/>
       <c r="H38" s="27"/>
     </row>
-    <row r="39" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1249,7 +1372,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="25"/>
     </row>
-    <row r="40" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="24">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1263,7 +1386,7 @@
       <c r="G40" s="26"/>
       <c r="H40" s="27"/>
     </row>
-    <row r="41" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1277,7 +1400,7 @@
       <c r="G41" s="19"/>
       <c r="H41" s="25"/>
     </row>
-    <row r="42" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="24">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1291,7 +1414,7 @@
       <c r="G42" s="26"/>
       <c r="H42" s="27"/>
     </row>
-    <row r="43" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="13">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -1305,7 +1428,7 @@
       <c r="G43" s="19"/>
       <c r="H43" s="25"/>
     </row>
-    <row r="44" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="24">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -1319,7 +1442,7 @@
       <c r="G44" s="26"/>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -1333,7 +1456,7 @@
       <c r="G45" s="19"/>
       <c r="H45" s="25"/>
     </row>
-    <row r="46" spans="2:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:16" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="24">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -1347,8 +1470,8 @@
       <c r="G46" s="26"/>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="2:16" ht="10.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:16" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:16" ht="10.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:16" s="4" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="31" t="s">
         <v>7</v>
       </c>
@@ -1390,14 +1513,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.296875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="88.296875" style="29" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="29"/>
+    <col min="1" max="1" width="3.25" style="29" customWidth="1"/>
+    <col min="2" max="2" width="88.25" style="29" customWidth="1"/>
+    <col min="3" max="16384" width="10.75" style="29"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" ht="90" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
         <v>9</v>
       </c>

</xml_diff>